<commit_message>
Updated Strategic Logistic Board
</commit_message>
<xml_diff>
--- a/_templates/Strategic_Logistics_Board/Warehouse_Complaints_de.xlsx
+++ b/_templates/Strategic_Logistics_Board/Warehouse_Complaints_de.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiashaas/git/peakboard-templates/_templates/Strategic_Logistics_Board/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E203363-BA5C-FC49-9728-61865E2440B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769EBEBC-E01B-E04F-90D8-D8074DB84994}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-52000" yWindow="-3720" windowWidth="42920" windowHeight="28080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,21 +40,12 @@
     <t>19:18:40</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>12:23:43</t>
   </si>
   <si>
-    <t>Damaged package</t>
-  </si>
-  <si>
     <t>16:31:21</t>
   </si>
   <si>
-    <t>Too late</t>
-  </si>
-  <si>
     <t>4:47:22</t>
   </si>
   <si>
@@ -67,9 +58,6 @@
     <t>21:25:43</t>
   </si>
   <si>
-    <t>Missing parts</t>
-  </si>
-  <si>
     <t>17:16:46</t>
   </si>
   <si>
@@ -722,6 +710,18 @@
   </si>
   <si>
     <t xml:space="preserve"> 15 von 3 Posten waren unvollständig</t>
+  </si>
+  <si>
+    <t>Verpackung beschädigt</t>
+  </si>
+  <si>
+    <t>Verspätet</t>
+  </si>
+  <si>
+    <t>Fehlende Teile</t>
+  </si>
+  <si>
+    <t>Sonstiges</t>
   </si>
 </sst>
 </file>
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="J185" sqref="J185"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1100,7 +1100,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1120,10 +1120,10 @@
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
@@ -1131,16 +1131,16 @@
         <v>43760</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>300</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.15">
@@ -1148,16 +1148,16 @@
         <v>43759</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>200</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.15">
@@ -1165,16 +1165,16 @@
         <v>43758</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>400</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E5" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
@@ -1182,16 +1182,16 @@
         <v>43757</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E6" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.15">
@@ -1199,16 +1199,16 @@
         <v>43756</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>400</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E7" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.15">
@@ -1216,16 +1216,16 @@
         <v>43755</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <v>400</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E8" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.15">
@@ -1233,16 +1233,16 @@
         <v>43754</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>300</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E9" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
@@ -1250,16 +1250,16 @@
         <v>43753</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>400</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E10" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
@@ -1267,16 +1267,16 @@
         <v>43752</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>400</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E11" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
@@ -1284,16 +1284,16 @@
         <v>43751</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>300</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E12" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.15">
@@ -1301,16 +1301,16 @@
         <v>43750</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C13">
         <v>400</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E13" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.15">
@@ -1318,16 +1318,16 @@
         <v>43749</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C14">
         <v>300</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E14" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.15">
@@ -1335,16 +1335,16 @@
         <v>43748</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C15">
         <v>400</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E15" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.15">
@@ -1352,16 +1352,16 @@
         <v>43747</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C16">
         <v>100</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E16" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.15">
@@ -1369,16 +1369,16 @@
         <v>43746</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C17">
         <v>400</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E17" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
@@ -1386,16 +1386,16 @@
         <v>43745</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E18" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
@@ -1403,16 +1403,16 @@
         <v>43744</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C19">
         <v>200</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E19" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.15">
@@ -1420,16 +1420,16 @@
         <v>43743</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C20">
         <v>400</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E20" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
@@ -1437,16 +1437,16 @@
         <v>43742</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>400</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E21" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -1454,16 +1454,16 @@
         <v>43741</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C22">
         <v>400</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E22" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -1471,16 +1471,16 @@
         <v>43740</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C23">
         <v>400</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E23" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
@@ -1488,16 +1488,16 @@
         <v>43739</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C24">
         <v>100</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E24" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
@@ -1505,16 +1505,16 @@
         <v>43738</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C25">
         <v>300</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E25" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
@@ -1522,16 +1522,16 @@
         <v>43737</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C26">
         <v>100</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E26" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
@@ -1539,16 +1539,16 @@
         <v>43736</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C27">
         <v>200</v>
       </c>
       <c r="D27" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E27" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
@@ -1556,16 +1556,16 @@
         <v>43735</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C28">
         <v>400</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E28" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -1573,16 +1573,16 @@
         <v>43734</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C29">
         <v>400</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E29" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
@@ -1590,16 +1590,16 @@
         <v>43733</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>400</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E30" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
@@ -1607,16 +1607,16 @@
         <v>43732</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C31">
         <v>300</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E31" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
@@ -1624,16 +1624,16 @@
         <v>43731</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C32">
         <v>200</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E32" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
@@ -1641,16 +1641,16 @@
         <v>43730</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C33">
         <v>300</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E33" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
@@ -1658,16 +1658,16 @@
         <v>43729</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C34">
         <v>400</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E34" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
@@ -1675,16 +1675,16 @@
         <v>43728</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C35">
         <v>400</v>
       </c>
       <c r="D35" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E35" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
@@ -1692,16 +1692,16 @@
         <v>43727</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C36">
         <v>400</v>
       </c>
       <c r="D36" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E36" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
@@ -1709,16 +1709,16 @@
         <v>43726</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C37">
         <v>400</v>
       </c>
       <c r="D37" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E37" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
@@ -1726,16 +1726,16 @@
         <v>43725</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C38">
         <v>400</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E38" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
@@ -1743,16 +1743,16 @@
         <v>43724</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C39">
         <v>400</v>
       </c>
       <c r="D39" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E39" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
@@ -1760,16 +1760,16 @@
         <v>43723</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C40">
         <v>200</v>
       </c>
       <c r="D40" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E40" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
@@ -1777,16 +1777,16 @@
         <v>43722</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C41">
         <v>400</v>
       </c>
       <c r="D41" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E41" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
@@ -1794,16 +1794,16 @@
         <v>43721</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C42">
         <v>400</v>
       </c>
       <c r="D42" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E42" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
@@ -1811,16 +1811,16 @@
         <v>43720</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C43">
         <v>400</v>
       </c>
       <c r="D43" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E43" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
@@ -1828,16 +1828,16 @@
         <v>43719</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C44">
         <v>200</v>
       </c>
       <c r="D44" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E44" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.15">
@@ -1845,16 +1845,16 @@
         <v>43718</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C45">
         <v>300</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E45" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
@@ -1862,16 +1862,16 @@
         <v>43717</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C46">
         <v>100</v>
       </c>
       <c r="D46" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E46" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
@@ -1879,16 +1879,16 @@
         <v>43716</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C47">
         <v>200</v>
       </c>
       <c r="D47" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E47" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
@@ -1896,16 +1896,16 @@
         <v>43715</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C48">
         <v>400</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E48" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
@@ -1913,16 +1913,16 @@
         <v>43714</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C49">
         <v>400</v>
       </c>
       <c r="D49" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E49" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
@@ -1930,16 +1930,16 @@
         <v>43713</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C50">
         <v>200</v>
       </c>
       <c r="D50" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E50" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.15">
@@ -1947,16 +1947,16 @@
         <v>43712</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C51">
         <v>400</v>
       </c>
       <c r="D51" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E51" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
@@ -1964,16 +1964,16 @@
         <v>43711</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C52">
         <v>400</v>
       </c>
       <c r="D52" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E52" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
@@ -1981,16 +1981,16 @@
         <v>43710</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C53">
         <v>400</v>
       </c>
       <c r="D53" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E53" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
@@ -1998,16 +1998,16 @@
         <v>43709</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C54">
         <v>300</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E54" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
@@ -2015,16 +2015,16 @@
         <v>43708</v>
       </c>
       <c r="B55" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C55">
         <v>400</v>
       </c>
       <c r="D55" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E55" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
@@ -2032,16 +2032,16 @@
         <v>43707</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C56">
         <v>400</v>
       </c>
       <c r="D56" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E56" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
@@ -2049,16 +2049,16 @@
         <v>43706</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C57">
         <v>400</v>
       </c>
       <c r="D57" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E57" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
@@ -2066,16 +2066,16 @@
         <v>43705</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C58">
         <v>300</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E58" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
@@ -2083,16 +2083,16 @@
         <v>43704</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C59">
         <v>400</v>
       </c>
       <c r="D59" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E59" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
@@ -2100,16 +2100,16 @@
         <v>43703</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C60">
         <v>400</v>
       </c>
       <c r="D60" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E60" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
@@ -2117,16 +2117,16 @@
         <v>43702</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C61">
         <v>400</v>
       </c>
       <c r="D61" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E61" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
@@ -2134,16 +2134,16 @@
         <v>43701</v>
       </c>
       <c r="B62" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C62">
         <v>400</v>
       </c>
       <c r="D62" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E62" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
@@ -2151,16 +2151,16 @@
         <v>43700</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C63">
         <v>200</v>
       </c>
       <c r="D63" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E63" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
@@ -2168,16 +2168,16 @@
         <v>43699</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C64">
         <v>400</v>
       </c>
       <c r="D64" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E64" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.15">
@@ -2185,16 +2185,16 @@
         <v>43698</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C65">
         <v>400</v>
       </c>
       <c r="D65" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E65" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
@@ -2202,16 +2202,16 @@
         <v>43697</v>
       </c>
       <c r="B66" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C66">
         <v>300</v>
       </c>
       <c r="D66" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E66" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
@@ -2219,16 +2219,16 @@
         <v>43696</v>
       </c>
       <c r="B67" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C67">
         <v>400</v>
       </c>
       <c r="D67" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E67" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
@@ -2236,16 +2236,16 @@
         <v>43695</v>
       </c>
       <c r="B68" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C68">
         <v>200</v>
       </c>
       <c r="D68" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E68" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
@@ -2253,16 +2253,16 @@
         <v>43694</v>
       </c>
       <c r="B69" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C69">
         <v>400</v>
       </c>
       <c r="D69" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E69" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
@@ -2270,16 +2270,16 @@
         <v>43693</v>
       </c>
       <c r="B70" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C70">
         <v>300</v>
       </c>
       <c r="D70" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E70" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
@@ -2287,16 +2287,16 @@
         <v>43692</v>
       </c>
       <c r="B71" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C71">
         <v>400</v>
       </c>
       <c r="D71" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E71" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
@@ -2304,16 +2304,16 @@
         <v>43691</v>
       </c>
       <c r="B72" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C72">
         <v>400</v>
       </c>
       <c r="D72" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E72" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
@@ -2321,16 +2321,16 @@
         <v>43690</v>
       </c>
       <c r="B73" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C73">
         <v>400</v>
       </c>
       <c r="D73" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E73" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
@@ -2338,16 +2338,16 @@
         <v>43689</v>
       </c>
       <c r="B74" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C74">
         <v>300</v>
       </c>
       <c r="D74" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E74" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
@@ -2355,16 +2355,16 @@
         <v>43688</v>
       </c>
       <c r="B75" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C75">
         <v>200</v>
       </c>
       <c r="D75" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E75" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
@@ -2372,16 +2372,16 @@
         <v>43687</v>
       </c>
       <c r="B76" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C76">
         <v>400</v>
       </c>
       <c r="D76" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E76" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
@@ -2389,16 +2389,16 @@
         <v>43686</v>
       </c>
       <c r="B77" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C77">
         <v>200</v>
       </c>
       <c r="D77" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E77" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
@@ -2406,16 +2406,16 @@
         <v>43685</v>
       </c>
       <c r="B78" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C78">
         <v>400</v>
       </c>
       <c r="D78" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E78" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
@@ -2423,16 +2423,16 @@
         <v>43684</v>
       </c>
       <c r="B79" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C79">
         <v>300</v>
       </c>
       <c r="D79" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E79" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
@@ -2440,16 +2440,16 @@
         <v>43683</v>
       </c>
       <c r="B80" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C80">
         <v>200</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E80" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
@@ -2457,16 +2457,16 @@
         <v>43682</v>
       </c>
       <c r="B81" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C81">
         <v>400</v>
       </c>
       <c r="D81" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E81" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
@@ -2474,16 +2474,16 @@
         <v>43681</v>
       </c>
       <c r="B82" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C82">
         <v>400</v>
       </c>
       <c r="D82" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E82" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
@@ -2491,16 +2491,16 @@
         <v>43680</v>
       </c>
       <c r="B83" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C83">
         <v>300</v>
       </c>
       <c r="D83" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E83" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
@@ -2508,16 +2508,16 @@
         <v>43679</v>
       </c>
       <c r="B84" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C84">
         <v>400</v>
       </c>
       <c r="D84" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E84" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
@@ -2525,16 +2525,16 @@
         <v>43678</v>
       </c>
       <c r="B85" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C85">
         <v>400</v>
       </c>
       <c r="D85" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E85" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
@@ -2542,16 +2542,16 @@
         <v>43677</v>
       </c>
       <c r="B86" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C86">
         <v>400</v>
       </c>
       <c r="D86" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E86" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.15">
@@ -2559,16 +2559,16 @@
         <v>43676</v>
       </c>
       <c r="B87" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C87">
         <v>400</v>
       </c>
       <c r="D87" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E87" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.15">
@@ -2576,16 +2576,16 @@
         <v>43675</v>
       </c>
       <c r="B88" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C88">
         <v>200</v>
       </c>
       <c r="D88" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E88" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.15">
@@ -2593,16 +2593,16 @@
         <v>43674</v>
       </c>
       <c r="B89" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C89">
         <v>400</v>
       </c>
       <c r="D89" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E89" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
@@ -2610,16 +2610,16 @@
         <v>43673</v>
       </c>
       <c r="B90" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C90">
         <v>200</v>
       </c>
       <c r="D90" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E90" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.15">
@@ -2627,16 +2627,16 @@
         <v>43672</v>
       </c>
       <c r="B91" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C91">
         <v>400</v>
       </c>
       <c r="D91" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E91" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
@@ -2644,16 +2644,16 @@
         <v>43671</v>
       </c>
       <c r="B92" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C92">
         <v>400</v>
       </c>
       <c r="D92" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E92" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
@@ -2661,16 +2661,16 @@
         <v>43670</v>
       </c>
       <c r="B93" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C93">
         <v>400</v>
       </c>
       <c r="D93" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E93" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.15">
@@ -2678,16 +2678,16 @@
         <v>43669</v>
       </c>
       <c r="B94" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C94">
         <v>200</v>
       </c>
       <c r="D94" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E94" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.15">
@@ -2695,16 +2695,16 @@
         <v>43668</v>
       </c>
       <c r="B95" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C95">
         <v>400</v>
       </c>
       <c r="D95" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E95" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.15">
@@ -2712,16 +2712,16 @@
         <v>43667</v>
       </c>
       <c r="B96" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C96">
         <v>400</v>
       </c>
       <c r="D96" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E96" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.15">
@@ -2729,16 +2729,16 @@
         <v>43666</v>
       </c>
       <c r="B97" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C97">
         <v>400</v>
       </c>
       <c r="D97" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E97" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.15">
@@ -2746,16 +2746,16 @@
         <v>43665</v>
       </c>
       <c r="B98" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C98">
         <v>200</v>
       </c>
       <c r="D98" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E98" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.15">
@@ -2763,16 +2763,16 @@
         <v>43664</v>
       </c>
       <c r="B99" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C99">
         <v>100</v>
       </c>
       <c r="D99" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E99" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.15">
@@ -2780,16 +2780,16 @@
         <v>43663</v>
       </c>
       <c r="B100" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C100">
         <v>300</v>
       </c>
       <c r="D100" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E100" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.15">
@@ -2797,16 +2797,16 @@
         <v>43662</v>
       </c>
       <c r="B101" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C101">
         <v>400</v>
       </c>
       <c r="D101" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E101" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.15">
@@ -2814,16 +2814,16 @@
         <v>43661</v>
       </c>
       <c r="B102" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C102">
         <v>100</v>
       </c>
       <c r="D102" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E102" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.15">
@@ -2831,16 +2831,16 @@
         <v>43660</v>
       </c>
       <c r="B103" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C103">
         <v>300</v>
       </c>
       <c r="D103" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E103" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.15">
@@ -2848,16 +2848,16 @@
         <v>43659</v>
       </c>
       <c r="B104" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C104">
         <v>300</v>
       </c>
       <c r="D104" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E104" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.15">
@@ -2865,16 +2865,16 @@
         <v>43658</v>
       </c>
       <c r="B105" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C105">
         <v>400</v>
       </c>
       <c r="D105" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E105" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.15">
@@ -2882,16 +2882,16 @@
         <v>43657</v>
       </c>
       <c r="B106" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C106">
         <v>300</v>
       </c>
       <c r="D106" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E106" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.15">
@@ -2899,16 +2899,16 @@
         <v>43656</v>
       </c>
       <c r="B107" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C107">
         <v>100</v>
       </c>
       <c r="D107" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E107" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.15">
@@ -2916,16 +2916,16 @@
         <v>43655</v>
       </c>
       <c r="B108" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C108">
         <v>100</v>
       </c>
       <c r="D108" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E108" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.15">
@@ -2933,16 +2933,16 @@
         <v>43654</v>
       </c>
       <c r="B109" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C109">
         <v>100</v>
       </c>
       <c r="D109" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E109" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.15">
@@ -2950,16 +2950,16 @@
         <v>43653</v>
       </c>
       <c r="B110" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C110">
         <v>200</v>
       </c>
       <c r="D110" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E110" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.15">
@@ -2967,16 +2967,16 @@
         <v>43652</v>
       </c>
       <c r="B111" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C111">
         <v>300</v>
       </c>
       <c r="D111" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E111" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.15">
@@ -2984,16 +2984,16 @@
         <v>43651</v>
       </c>
       <c r="B112" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C112">
         <v>300</v>
       </c>
       <c r="D112" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E112" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.15">
@@ -3001,16 +3001,16 @@
         <v>43650</v>
       </c>
       <c r="B113" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C113">
         <v>300</v>
       </c>
       <c r="D113" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E113" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.15">
@@ -3018,16 +3018,16 @@
         <v>43649</v>
       </c>
       <c r="B114" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C114">
         <v>100</v>
       </c>
       <c r="D114" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E114" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.15">
@@ -3035,16 +3035,16 @@
         <v>43648</v>
       </c>
       <c r="B115" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C115">
         <v>300</v>
       </c>
       <c r="D115" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E115" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.15">
@@ -3052,16 +3052,16 @@
         <v>43647</v>
       </c>
       <c r="B116" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C116">
         <v>400</v>
       </c>
       <c r="D116" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E116" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.15">
@@ -3069,16 +3069,16 @@
         <v>43646</v>
       </c>
       <c r="B117" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C117">
         <v>400</v>
       </c>
       <c r="D117" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E117" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.15">
@@ -3086,16 +3086,16 @@
         <v>43645</v>
       </c>
       <c r="B118" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C118">
         <v>400</v>
       </c>
       <c r="D118" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E118" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.15">
@@ -3103,16 +3103,16 @@
         <v>43644</v>
       </c>
       <c r="B119" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C119">
         <v>400</v>
       </c>
       <c r="D119" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E119" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.15">
@@ -3120,16 +3120,16 @@
         <v>43643</v>
       </c>
       <c r="B120" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C120">
         <v>200</v>
       </c>
       <c r="D120" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E120" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.15">
@@ -3137,16 +3137,16 @@
         <v>43642</v>
       </c>
       <c r="B121" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C121">
         <v>400</v>
       </c>
       <c r="D121" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E121" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.15">
@@ -3154,16 +3154,16 @@
         <v>43641</v>
       </c>
       <c r="B122" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C122">
         <v>400</v>
       </c>
       <c r="D122" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E122" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.15">
@@ -3171,16 +3171,16 @@
         <v>43640</v>
       </c>
       <c r="B123" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C123">
         <v>200</v>
       </c>
       <c r="D123" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E123" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.15">
@@ -3188,16 +3188,16 @@
         <v>43639</v>
       </c>
       <c r="B124" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C124">
         <v>100</v>
       </c>
       <c r="D124" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E124" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.15">
@@ -3205,16 +3205,16 @@
         <v>43638</v>
       </c>
       <c r="B125" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C125">
         <v>200</v>
       </c>
       <c r="D125" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E125" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.15">
@@ -3222,16 +3222,16 @@
         <v>43637</v>
       </c>
       <c r="B126" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C126">
         <v>200</v>
       </c>
       <c r="D126" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E126" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.15">
@@ -3239,16 +3239,16 @@
         <v>43636</v>
       </c>
       <c r="B127" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C127">
         <v>100</v>
       </c>
       <c r="D127" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E127" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.15">
@@ -3256,16 +3256,16 @@
         <v>43635</v>
       </c>
       <c r="B128" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C128">
         <v>300</v>
       </c>
       <c r="D128" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E128" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.15">
@@ -3273,16 +3273,16 @@
         <v>43634</v>
       </c>
       <c r="B129" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C129">
         <v>200</v>
       </c>
       <c r="D129" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E129" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.15">
@@ -3290,16 +3290,16 @@
         <v>43633</v>
       </c>
       <c r="B130" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C130">
         <v>300</v>
       </c>
       <c r="D130" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E130" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.15">
@@ -3307,16 +3307,16 @@
         <v>43632</v>
       </c>
       <c r="B131" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C131">
         <v>300</v>
       </c>
       <c r="D131" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E131" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.15">
@@ -3324,16 +3324,16 @@
         <v>43631</v>
       </c>
       <c r="B132" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C132">
         <v>400</v>
       </c>
       <c r="D132" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E132" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.15">
@@ -3341,16 +3341,16 @@
         <v>43630</v>
       </c>
       <c r="B133" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C133">
         <v>300</v>
       </c>
       <c r="D133" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E133" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.15">
@@ -3358,16 +3358,16 @@
         <v>43629</v>
       </c>
       <c r="B134" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C134">
         <v>100</v>
       </c>
       <c r="D134" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E134" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.15">
@@ -3375,16 +3375,16 @@
         <v>43628</v>
       </c>
       <c r="B135" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C135">
         <v>100</v>
       </c>
       <c r="D135" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E135" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.15">
@@ -3392,16 +3392,16 @@
         <v>43627</v>
       </c>
       <c r="B136" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C136">
         <v>400</v>
       </c>
       <c r="D136" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E136" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.15">
@@ -3409,16 +3409,16 @@
         <v>43626</v>
       </c>
       <c r="B137" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C137">
         <v>400</v>
       </c>
       <c r="D137" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E137" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.15">
@@ -3426,16 +3426,16 @@
         <v>43625</v>
       </c>
       <c r="B138" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C138">
         <v>200</v>
       </c>
       <c r="D138" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E138" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.15">
@@ -3443,16 +3443,16 @@
         <v>43624</v>
       </c>
       <c r="B139" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C139">
         <v>100</v>
       </c>
       <c r="D139" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E139" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.15">
@@ -3460,16 +3460,16 @@
         <v>43623</v>
       </c>
       <c r="B140" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C140">
         <v>100</v>
       </c>
       <c r="D140" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E140" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.15">
@@ -3477,16 +3477,16 @@
         <v>43622</v>
       </c>
       <c r="B141" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C141">
         <v>100</v>
       </c>
       <c r="D141" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E141" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.15">
@@ -3494,16 +3494,16 @@
         <v>43621</v>
       </c>
       <c r="B142" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C142">
         <v>200</v>
       </c>
       <c r="D142" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E142" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.15">
@@ -3511,16 +3511,16 @@
         <v>43620</v>
       </c>
       <c r="B143" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C143">
         <v>400</v>
       </c>
       <c r="D143" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E143" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.15">
@@ -3528,16 +3528,16 @@
         <v>43619</v>
       </c>
       <c r="B144" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C144">
         <v>200</v>
       </c>
       <c r="D144" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E144" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.15">
@@ -3545,16 +3545,16 @@
         <v>43618</v>
       </c>
       <c r="B145" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C145">
         <v>200</v>
       </c>
       <c r="D145" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E145" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.15">
@@ -3562,16 +3562,16 @@
         <v>43617</v>
       </c>
       <c r="B146" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C146">
         <v>100</v>
       </c>
       <c r="D146" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E146" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.15">
@@ -3579,16 +3579,16 @@
         <v>43616</v>
       </c>
       <c r="B147" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C147">
         <v>200</v>
       </c>
       <c r="D147" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E147" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.15">
@@ -3596,16 +3596,16 @@
         <v>43615</v>
       </c>
       <c r="B148" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C148">
         <v>300</v>
       </c>
       <c r="D148" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E148" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.15">
@@ -3613,16 +3613,16 @@
         <v>43614</v>
       </c>
       <c r="B149" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C149">
         <v>400</v>
       </c>
       <c r="D149" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E149" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.15">
@@ -3630,16 +3630,16 @@
         <v>43613</v>
       </c>
       <c r="B150" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C150">
         <v>400</v>
       </c>
       <c r="D150" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E150" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.15">
@@ -3647,16 +3647,16 @@
         <v>43612</v>
       </c>
       <c r="B151" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C151">
         <v>400</v>
       </c>
       <c r="D151" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E151" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.15">
@@ -3664,16 +3664,16 @@
         <v>43611</v>
       </c>
       <c r="B152" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C152">
         <v>300</v>
       </c>
       <c r="D152" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E152" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.15">
@@ -3681,16 +3681,16 @@
         <v>43610</v>
       </c>
       <c r="B153" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C153">
         <v>400</v>
       </c>
       <c r="D153" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E153" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.15">
@@ -3698,16 +3698,16 @@
         <v>43609</v>
       </c>
       <c r="B154" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C154">
         <v>300</v>
       </c>
       <c r="D154" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E154" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.15">
@@ -3715,16 +3715,16 @@
         <v>43608</v>
       </c>
       <c r="B155" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C155">
         <v>300</v>
       </c>
       <c r="D155" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E155" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.15">
@@ -3732,16 +3732,16 @@
         <v>43607</v>
       </c>
       <c r="B156" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C156">
         <v>300</v>
       </c>
       <c r="D156" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E156" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.15">
@@ -3749,16 +3749,16 @@
         <v>43606</v>
       </c>
       <c r="B157" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C157">
         <v>200</v>
       </c>
       <c r="D157" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E157" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.15">
@@ -3766,16 +3766,16 @@
         <v>43605</v>
       </c>
       <c r="B158" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C158">
         <v>100</v>
       </c>
       <c r="D158" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E158" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.15">
@@ -3783,16 +3783,16 @@
         <v>43604</v>
       </c>
       <c r="B159" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C159">
         <v>100</v>
       </c>
       <c r="D159" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E159" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.15">
@@ -3800,16 +3800,16 @@
         <v>43603</v>
       </c>
       <c r="B160" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C160">
         <v>200</v>
       </c>
       <c r="D160" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E160" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.15">
@@ -3817,16 +3817,16 @@
         <v>43602</v>
       </c>
       <c r="B161" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C161">
         <v>400</v>
       </c>
       <c r="D161" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E161" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.15">
@@ -3834,16 +3834,16 @@
         <v>43601</v>
       </c>
       <c r="B162" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C162">
         <v>100</v>
       </c>
       <c r="D162" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E162" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.15">
@@ -3851,16 +3851,16 @@
         <v>43600</v>
       </c>
       <c r="B163" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C163">
         <v>100</v>
       </c>
       <c r="D163" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E163" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.15">
@@ -3868,16 +3868,16 @@
         <v>43599</v>
       </c>
       <c r="B164" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C164">
         <v>100</v>
       </c>
       <c r="D164" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E164" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.15">
@@ -3885,16 +3885,16 @@
         <v>43598</v>
       </c>
       <c r="B165" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C165">
         <v>200</v>
       </c>
       <c r="D165" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E165" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.15">
@@ -3902,16 +3902,16 @@
         <v>43597</v>
       </c>
       <c r="B166" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C166">
         <v>100</v>
       </c>
       <c r="D166" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E166" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.15">
@@ -3919,16 +3919,16 @@
         <v>43596</v>
       </c>
       <c r="B167" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C167">
         <v>200</v>
       </c>
       <c r="D167" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E167" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.15">
@@ -3936,16 +3936,16 @@
         <v>43595</v>
       </c>
       <c r="B168" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C168">
         <v>100</v>
       </c>
       <c r="D168" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E168" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.15">
@@ -3953,16 +3953,16 @@
         <v>43594</v>
       </c>
       <c r="B169" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C169">
         <v>300</v>
       </c>
       <c r="D169" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E169" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.15">
@@ -3970,16 +3970,16 @@
         <v>43593</v>
       </c>
       <c r="B170" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C170">
         <v>300</v>
       </c>
       <c r="D170" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E170" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.15">
@@ -3987,16 +3987,16 @@
         <v>43592</v>
       </c>
       <c r="B171" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C171">
         <v>100</v>
       </c>
       <c r="D171" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E171" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.15">
@@ -4004,16 +4004,16 @@
         <v>43591</v>
       </c>
       <c r="B172" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C172">
         <v>100</v>
       </c>
       <c r="D172" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E172" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.15">
@@ -4021,16 +4021,16 @@
         <v>43590</v>
       </c>
       <c r="B173" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C173">
         <v>200</v>
       </c>
       <c r="D173" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E173" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.15">
@@ -4038,16 +4038,16 @@
         <v>43589</v>
       </c>
       <c r="B174" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C174">
         <v>100</v>
       </c>
       <c r="D174" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E174" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.15">
@@ -4055,16 +4055,16 @@
         <v>43588</v>
       </c>
       <c r="B175" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C175">
         <v>400</v>
       </c>
       <c r="D175" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E175" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.15">
@@ -4072,16 +4072,16 @@
         <v>43587</v>
       </c>
       <c r="B176" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C176">
         <v>100</v>
       </c>
       <c r="D176" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E176" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.15">
@@ -4089,16 +4089,16 @@
         <v>43586</v>
       </c>
       <c r="B177" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C177">
         <v>100</v>
       </c>
       <c r="D177" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E177" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.15">
@@ -4106,16 +4106,16 @@
         <v>43585</v>
       </c>
       <c r="B178" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C178">
         <v>100</v>
       </c>
       <c r="D178" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E178" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.15">
@@ -4123,16 +4123,16 @@
         <v>43584</v>
       </c>
       <c r="B179" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C179">
         <v>200</v>
       </c>
       <c r="D179" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E179" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.15">
@@ -4140,16 +4140,16 @@
         <v>43583</v>
       </c>
       <c r="B180" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C180">
         <v>100</v>
       </c>
       <c r="D180" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E180" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.15">
@@ -4157,16 +4157,16 @@
         <v>43582</v>
       </c>
       <c r="B181" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C181">
         <v>300</v>
       </c>
       <c r="D181" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E181" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.15">
@@ -4174,16 +4174,16 @@
         <v>43581</v>
       </c>
       <c r="B182" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C182">
         <v>300</v>
       </c>
       <c r="D182" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E182" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.15">
@@ -4191,16 +4191,16 @@
         <v>43580</v>
       </c>
       <c r="B183" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C183">
         <v>100</v>
       </c>
       <c r="D183" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E183" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.15">
@@ -4208,16 +4208,16 @@
         <v>43579</v>
       </c>
       <c r="B184" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C184">
         <v>300</v>
       </c>
       <c r="D184" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E184" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.15">
@@ -4225,16 +4225,16 @@
         <v>43578</v>
       </c>
       <c r="B185" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C185">
         <v>100</v>
       </c>
       <c r="D185" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E185" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.15">
@@ -4242,16 +4242,16 @@
         <v>43577</v>
       </c>
       <c r="B186" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C186">
         <v>400</v>
       </c>
       <c r="D186" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E186" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.15">
@@ -4259,16 +4259,16 @@
         <v>43576</v>
       </c>
       <c r="B187" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C187">
         <v>100</v>
       </c>
       <c r="D187" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E187" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.15">
@@ -4276,16 +4276,16 @@
         <v>43575</v>
       </c>
       <c r="B188" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C188">
         <v>300</v>
       </c>
       <c r="D188" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E188" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.15">
@@ -4293,16 +4293,16 @@
         <v>43574</v>
       </c>
       <c r="B189" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C189">
         <v>200</v>
       </c>
       <c r="D189" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E189" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.15">
@@ -4310,16 +4310,16 @@
         <v>43573</v>
       </c>
       <c r="B190" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C190">
         <v>300</v>
       </c>
       <c r="D190" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E190" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.15">
@@ -4327,16 +4327,16 @@
         <v>43572</v>
       </c>
       <c r="B191" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C191">
         <v>400</v>
       </c>
       <c r="D191" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E191" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.15">
@@ -4344,16 +4344,16 @@
         <v>43571</v>
       </c>
       <c r="B192" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C192">
         <v>100</v>
       </c>
       <c r="D192" t="s">
-        <v>5</v>
+        <v>232</v>
       </c>
       <c r="E192" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.15">
@@ -4361,16 +4361,16 @@
         <v>43570</v>
       </c>
       <c r="B193" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C193">
         <v>200</v>
       </c>
       <c r="D193" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E193" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.15">
@@ -4378,16 +4378,16 @@
         <v>43569</v>
       </c>
       <c r="B194" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C194">
         <v>400</v>
       </c>
       <c r="D194" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E194" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.15">
@@ -4395,16 +4395,16 @@
         <v>43568</v>
       </c>
       <c r="B195" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C195">
         <v>200</v>
       </c>
       <c r="D195" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E195" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.15">
@@ -4412,16 +4412,16 @@
         <v>43567</v>
       </c>
       <c r="B196" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C196">
         <v>300</v>
       </c>
       <c r="D196" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E196" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.15">
@@ -4429,16 +4429,16 @@
         <v>43566</v>
       </c>
       <c r="B197" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C197">
         <v>300</v>
       </c>
       <c r="D197" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E197" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.15">
@@ -4446,16 +4446,16 @@
         <v>43565</v>
       </c>
       <c r="B198" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C198">
         <v>200</v>
       </c>
       <c r="D198" t="s">
-        <v>9</v>
+        <v>230</v>
       </c>
       <c r="E198" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.15">
@@ -4463,16 +4463,16 @@
         <v>43564</v>
       </c>
       <c r="B199" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C199">
         <v>400</v>
       </c>
       <c r="D199" t="s">
-        <v>14</v>
+        <v>231</v>
       </c>
       <c r="E199" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.15">
@@ -4480,20 +4480,19 @@
         <v>43563</v>
       </c>
       <c r="B200" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C200">
         <v>300</v>
       </c>
       <c r="D200" t="s">
-        <v>7</v>
+        <v>229</v>
       </c>
       <c r="E200" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E200" xr:uid="{C6C7FBCD-F692-6B42-AB1F-A7FA4327338B}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>